<commit_message>
finsihed variant comparison pathway enrichment graph
</commit_message>
<xml_diff>
--- a/Outputs/Mummichog Outputs/clades_mummichog.xlsx
+++ b/Outputs/Mummichog Outputs/clades_mummichog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/jdprest_emory_edu/Documents/Research/Manuscripts and Projects/Active Projects/Thyroid Metabolomics/DTC-metabolomics-2025/Outputs/Mummichog Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{F7DDF023-177B-D747-AFBC-F9B761A98FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1ACAF51-FDCD-664D-8363-3919D25CF810}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{F7DDF023-177B-D747-AFBC-F9B761A98FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAB2AF9F-8884-F647-A4F2-387326BB9FB9}"/>
   <bookViews>
-    <workbookView xWindow="39400" yWindow="-2080" windowWidth="17820" windowHeight="17640" activeTab="1" xr2:uid="{C6B41103-796F-6E47-BFBD-4F4096F04FFA}"/>
+    <workbookView xWindow="39400" yWindow="-2080" windowWidth="17820" windowHeight="17640" xr2:uid="{C6B41103-796F-6E47-BFBD-4F4096F04FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="EnrichNet" sheetId="1" r:id="rId1"/>
@@ -1408,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46434FA-F8B0-5948-89B1-27BFBAA6F66B}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1437,38 +1437,38 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2">
-        <v>1.8646E-4</v>
+        <v>4.8811000000000002E-3</v>
       </c>
       <c r="D2" s="1">
-        <v>4.0071000000000004E-3</v>
+        <v>4.0685000000000001E-3</v>
       </c>
       <c r="E2" s="3">
         <f>-LOG10(C2)</f>
-        <v>3.7294143201151755</v>
+        <v>2.3114822947808249</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2">
-        <v>3.5765999999999999E-4</v>
+        <v>4.9807000000000002E-3</v>
       </c>
       <c r="D3" s="1">
-        <v>4.0093000000000004E-3</v>
+        <v>4.0698000000000002E-3</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E21" si="0">-LOG10(C3)</f>
-        <v>3.4465296277868789</v>
+        <f>-LOG10(C3)</f>
+        <v>2.3027096161211178</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1485,318 +1485,322 @@
         <v>4.0100999999999999E-3</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="0"/>
+        <f>-LOG10(C4)</f>
         <v>3.3790523544407765</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2">
-        <v>2.2271000000000001E-3</v>
+        <v>4.7124999999999997E-3</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0337000000000003E-3</v>
+        <v>4.0663000000000001E-3</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
-        <v>2.6522602820799479</v>
+        <f>-LOG10(C5)</f>
+        <v>2.3267486367861507</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2">
-        <v>2.9036999999999999E-3</v>
+        <v>3.1364000000000001E-3</v>
       </c>
       <c r="D6" s="1">
-        <v>4.0425000000000001E-3</v>
+        <v>4.0455999999999999E-3</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
-        <v>2.5370482554219453</v>
+        <f>-LOG10(C6)</f>
+        <v>2.5035685548158</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>30</v>
       </c>
       <c r="C7" s="2">
-        <v>3.1364000000000001E-3</v>
+        <v>1.1635E-2</v>
       </c>
       <c r="D7" s="1">
-        <v>4.0455999999999999E-3</v>
+        <v>4.1587000000000004E-3</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="0"/>
-        <v>2.5035685548158</v>
+        <f>-LOG10(C7)</f>
+        <v>1.9342336123772512</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2">
-        <v>3.5726E-3</v>
+        <v>2.4031E-2</v>
       </c>
       <c r="D8" s="1">
-        <v>4.0512999999999999E-3</v>
+        <v>4.3290000000000004E-3</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="0"/>
-        <v>2.4470156061086166</v>
+        <f>-LOG10(C8)</f>
+        <v>1.6192281565599931</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2">
-        <v>4.7124999999999997E-3</v>
+        <v>1.4463E-2</v>
       </c>
       <c r="D9" s="1">
-        <v>4.0663000000000001E-3</v>
+        <v>4.1970000000000002E-3</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="0"/>
-        <v>2.3267486367861507</v>
+        <f>-LOG10(C9)</f>
+        <v>1.8397416137973306</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2">
-        <v>4.8811000000000002E-3</v>
+        <v>2.1808000000000001E-2</v>
       </c>
       <c r="D10" s="1">
-        <v>4.0685000000000001E-3</v>
+        <v>4.2984E-3</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="0"/>
-        <v>2.3114822947808249</v>
+        <f>-LOG10(C10)</f>
+        <v>1.6613841615094016</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2">
-        <v>4.9807000000000002E-3</v>
+        <v>2.9036999999999999E-3</v>
       </c>
       <c r="D11" s="1">
-        <v>4.0698000000000002E-3</v>
+        <v>4.0425000000000001E-3</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="0"/>
-        <v>2.3027096161211178</v>
+        <f>-LOG10(C11)</f>
+        <v>2.5370482554219453</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2">
-        <v>8.2024000000000003E-3</v>
+        <v>2.0489E-2</v>
       </c>
       <c r="D12" s="1">
-        <v>4.1126000000000001E-3</v>
+        <v>4.28E-3</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>2.0860590556341334</v>
+        <f>-LOG10(C12)</f>
+        <v>1.6884792375519513</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2">
-        <v>1.1635E-2</v>
+        <v>2.1984E-2</v>
       </c>
       <c r="D13" s="1">
-        <v>4.1587000000000004E-3</v>
+        <v>4.3008999999999999E-3</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="0"/>
-        <v>1.9342336123772512</v>
+        <f>-LOG10(C13)</f>
+        <v>1.6578932846205436</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2">
-        <v>1.1709000000000001E-2</v>
+        <v>2.2271000000000001E-3</v>
       </c>
       <c r="D14" s="1">
-        <v>4.1596999999999997E-3</v>
+        <v>4.0337000000000003E-3</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="0"/>
-        <v>1.9314801939990889</v>
+        <f>-LOG10(C14)</f>
+        <v>2.6522602820799479</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2">
-        <v>1.3122999999999999E-2</v>
+        <v>3.5726E-3</v>
       </c>
       <c r="D15" s="1">
-        <v>4.1787999999999999E-3</v>
+        <v>4.0512999999999999E-3</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="0"/>
-        <v>1.881966871171433</v>
+        <f>-LOG10(C15)</f>
+        <v>2.4470156061086166</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2">
-        <v>1.4463E-2</v>
+        <v>1.1709000000000001E-2</v>
       </c>
       <c r="D16" s="1">
-        <v>4.1970000000000002E-3</v>
+        <v>4.1596999999999997E-3</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="0"/>
-        <v>1.8397416137973306</v>
+        <f>-LOG10(C16)</f>
+        <v>1.9314801939990889</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2">
-        <v>1.4470999999999999E-2</v>
+        <v>8.2024000000000003E-3</v>
       </c>
       <c r="D17" s="1">
-        <v>4.1970999999999996E-3</v>
+        <v>4.1126000000000001E-3</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="0"/>
-        <v>1.839501456477654</v>
+        <f>-LOG10(C17)</f>
+        <v>2.0860590556341334</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2">
-        <v>2.0489E-2</v>
+        <v>1.8646E-4</v>
       </c>
       <c r="D18" s="1">
-        <v>4.28E-3</v>
+        <v>4.0071000000000004E-3</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6884792375519513</v>
+        <f>-LOG10(C18)</f>
+        <v>3.7294143201151755</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C19" s="2">
-        <v>2.1808000000000001E-2</v>
+        <v>3.5765999999999999E-4</v>
       </c>
       <c r="D19" s="1">
-        <v>4.2984E-3</v>
+        <v>4.0093000000000004E-3</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6613841615094016</v>
+        <f>-LOG10(C19)</f>
+        <v>3.4465296277868789</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C20" s="2">
-        <v>2.1984E-2</v>
+        <v>1.3122999999999999E-2</v>
       </c>
       <c r="D20" s="1">
-        <v>4.3008999999999999E-3</v>
+        <v>4.1787999999999999E-3</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6578932846205436</v>
+        <f>-LOG10(C20)</f>
+        <v>1.881966871171433</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2">
-        <v>2.4031E-2</v>
+        <v>1.4470999999999999E-2</v>
       </c>
       <c r="D21" s="1">
-        <v>4.3290000000000004E-3</v>
+        <v>4.1970999999999996E-3</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6192281565599931</v>
+        <f>-LOG10(C21)</f>
+        <v>1.839501456477654</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E21" xr:uid="{D46434FA-F8B0-5948-89B1-27BFBAA6F66B}"/>
+  <autoFilter ref="A1:E21" xr:uid="{D46434FA-F8B0-5948-89B1-27BFBAA6F66B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">
+      <sortCondition descending="1" ref="B1:B21"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1805,7 +1809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BACC2E1-2DBB-C649-8AEE-E0F3B43A4914}">
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>